<commit_message>
Include functios to fill Base Model Year and Projections files
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A-O_Demand.xlsx
+++ b/t1_confection/A1_Outputs/A-O_Demand.xlsx
@@ -721,12 +721,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELCCRIAR02</t>
+          <t>ELCCRIXX02</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica, in region AR.</t>
+          <t>Output demand of transmission lines in Costa Rica</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -753,94 +753,94 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>9.5</v>
+        <v>40.82</v>
       </c>
       <c r="J2" t="n">
-        <v>11.03</v>
+        <v>43.12</v>
       </c>
       <c r="K2" t="n">
-        <v>12.58</v>
+        <v>45.42</v>
       </c>
       <c r="L2" t="n">
-        <v>14.11</v>
+        <v>47.72</v>
       </c>
       <c r="M2" t="n">
-        <v>15.66</v>
+        <v>50.02</v>
       </c>
       <c r="N2" t="n">
-        <v>17.32</v>
+        <v>52.73</v>
       </c>
       <c r="O2" t="n">
-        <v>18.97</v>
+        <v>55.43</v>
       </c>
       <c r="P2" t="n">
-        <v>20.62</v>
+        <v>58.14</v>
       </c>
       <c r="Q2" t="n">
-        <v>22.27</v>
+        <v>60.84</v>
       </c>
       <c r="R2" t="n">
-        <v>23.95</v>
+        <v>63.55</v>
       </c>
       <c r="S2" t="n">
-        <v>25.73</v>
+        <v>66.51000000000001</v>
       </c>
       <c r="T2" t="n">
-        <v>27.51</v>
+        <v>69.48</v>
       </c>
       <c r="U2" t="n">
-        <v>29.28</v>
+        <v>72.44</v>
       </c>
       <c r="V2" t="n">
-        <v>31.09</v>
+        <v>75.40000000000001</v>
       </c>
       <c r="W2" t="n">
-        <v>32.86</v>
+        <v>78.36</v>
       </c>
       <c r="X2" t="n">
-        <v>34.84</v>
+        <v>81.70999999999999</v>
       </c>
       <c r="Y2" t="n">
-        <v>36.82</v>
+        <v>85.06</v>
       </c>
       <c r="Z2" t="n">
-        <v>38.8</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="AA2" t="n">
-        <v>40.78</v>
+        <v>91.75</v>
       </c>
       <c r="AB2" t="n">
-        <v>42.75</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="AC2" t="n">
-        <v>44.93</v>
+        <v>98.75</v>
       </c>
       <c r="AD2" t="n">
-        <v>47.11</v>
+        <v>102.39</v>
       </c>
       <c r="AE2" t="n">
-        <v>49.29</v>
+        <v>106.04</v>
       </c>
       <c r="AF2" t="n">
-        <v>51.47</v>
+        <v>109.68</v>
       </c>
       <c r="AG2" t="n">
-        <v>53.64</v>
+        <v>113.33</v>
       </c>
       <c r="AH2" t="n">
-        <v>56</v>
+        <v>117.16</v>
       </c>
       <c r="AI2" t="n">
-        <v>58.35</v>
+        <v>121</v>
       </c>
       <c r="AJ2" t="n">
-        <v>60.7</v>
+        <v>124.84</v>
       </c>
       <c r="AK2" t="n">
-        <v>63.06</v>
+        <v>128.67</v>
       </c>
       <c r="AL2" t="n">
-        <v>65.41</v>
+        <v>132.51</v>
       </c>
     </row>
     <row r="3">
@@ -851,12 +851,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ELCCRIXX02</t>
+          <t>ELCPANXX02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica</t>
+          <t>Output demand of transmission lines in Panama</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -883,94 +883,94 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>40.82</v>
+        <v>62.21</v>
       </c>
       <c r="J3" t="n">
-        <v>43.11</v>
+        <v>66.56999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>45.41</v>
+        <v>70.93000000000001</v>
       </c>
       <c r="L3" t="n">
-        <v>47.7</v>
+        <v>75.29000000000001</v>
       </c>
       <c r="M3" t="n">
-        <v>50</v>
+        <v>79.65000000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>52.7</v>
+        <v>84.16</v>
       </c>
       <c r="O3" t="n">
-        <v>55.41</v>
+        <v>88.66</v>
       </c>
       <c r="P3" t="n">
-        <v>58.11</v>
+        <v>93.17</v>
       </c>
       <c r="Q3" t="n">
-        <v>60.82</v>
+        <v>97.67</v>
       </c>
       <c r="R3" t="n">
-        <v>63.53</v>
+        <v>102.18</v>
       </c>
       <c r="S3" t="n">
-        <v>66.48999999999999</v>
+        <v>106.88</v>
       </c>
       <c r="T3" t="n">
-        <v>69.45</v>
+        <v>111.59</v>
       </c>
       <c r="U3" t="n">
-        <v>72.41</v>
+        <v>116.29</v>
       </c>
       <c r="V3" t="n">
-        <v>75.37</v>
+        <v>120.99</v>
       </c>
       <c r="W3" t="n">
-        <v>78.33</v>
+        <v>125.69</v>
       </c>
       <c r="X3" t="n">
-        <v>81.68000000000001</v>
+        <v>130.64</v>
       </c>
       <c r="Y3" t="n">
-        <v>85.03</v>
+        <v>135.58</v>
       </c>
       <c r="Z3" t="n">
-        <v>88.37</v>
+        <v>140.52</v>
       </c>
       <c r="AA3" t="n">
-        <v>91.72</v>
+        <v>145.46</v>
       </c>
       <c r="AB3" t="n">
-        <v>95.06999999999999</v>
+        <v>150.41</v>
       </c>
       <c r="AC3" t="n">
-        <v>98.70999999999999</v>
+        <v>155.74</v>
       </c>
       <c r="AD3" t="n">
-        <v>102.36</v>
+        <v>161.07</v>
       </c>
       <c r="AE3" t="n">
-        <v>106</v>
+        <v>166.4</v>
       </c>
       <c r="AF3" t="n">
-        <v>109.64</v>
+        <v>171.73</v>
       </c>
       <c r="AG3" t="n">
-        <v>113.29</v>
+        <v>177.07</v>
       </c>
       <c r="AH3" t="n">
-        <v>117.13</v>
+        <v>182.58</v>
       </c>
       <c r="AI3" t="n">
-        <v>120.96</v>
+        <v>188.1</v>
       </c>
       <c r="AJ3" t="n">
-        <v>124.8</v>
+        <v>193.62</v>
       </c>
       <c r="AK3" t="n">
-        <v>128.64</v>
+        <v>199.14</v>
       </c>
       <c r="AL3" t="n">
-        <v>132.47</v>
+        <v>204.66</v>
       </c>
     </row>
   </sheetData>
@@ -1202,12 +1202,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ELCCRIAR02</t>
+          <t>ELCCRIXX02</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica, in region AR.</t>
+          <t>Output demand of transmission lines in Costa Rica</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1234,94 +1234,94 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="K2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="L2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="M2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="N2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="O2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="P2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="R2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="S2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="T2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="U2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="V2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="W2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="X2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="3">
@@ -1337,12 +1337,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ELCCRIXX02</t>
+          <t>ELCPANXX02</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica</t>
+          <t>Output demand of transmission lines in Panama</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1369,94 +1369,94 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="L3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="M3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="N3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="O3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="P3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="R3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="S3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="T3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="U3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="V3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="W3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="X3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4">
@@ -1472,12 +1472,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ELCCRIAR02</t>
+          <t>ELCCRIXX02</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica, in region AR.</t>
+          <t>Output demand of transmission lines in Costa Rica</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1504,94 +1504,94 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="K4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="L4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="M4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="N4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="O4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="P4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="R4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="S4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="T4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="U4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="V4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="W4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="X4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="5">
@@ -1607,12 +1607,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ELCCRIXX02</t>
+          <t>ELCPANXX02</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica</t>
+          <t>Output demand of transmission lines in Panama</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1742,12 +1742,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ELCCRIAR02</t>
+          <t>ELCCRIXX02</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica, in region AR.</t>
+          <t>Output demand of transmission lines in Costa Rica</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1774,94 +1774,94 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="K6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="L6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="M6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="N6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="O6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="P6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="R6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="S6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="T6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="U6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="V6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="W6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="X6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="7">
@@ -1877,12 +1877,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ELCCRIXX02</t>
+          <t>ELCPANXX02</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica</t>
+          <t>Output demand of transmission lines in Panama</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2012,12 +2012,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ELCCRIAR02</t>
+          <t>ELCCRIXX02</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica, in region AR.</t>
+          <t>Output demand of transmission lines in Costa Rica</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2044,94 +2044,94 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="K8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="L8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="M8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="N8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="O8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="P8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="R8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="S8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="T8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="U8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="V8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="W8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="X8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="9">
@@ -2147,12 +2147,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ELCCRIXX02</t>
+          <t>ELCPANXX02</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Output demand of transmission lines in Costa Rica</t>
+          <t>Output demand of transmission lines in Panama</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2179,94 +2179,94 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="K9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="L9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="M9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="N9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="O9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="P9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="R9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="S9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="T9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="U9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="V9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="W9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="X9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>